<commit_message>
Update passenger rail data
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2531,6 +2531,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="47" fillId="33" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2566,30 +2590,6 @@
     </xf>
     <xf numFmtId="0" fontId="49" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3223,7 +3223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3667,99 +3667,99 @@
       <c r="R11" s="71"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="161" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="175" t="s">
+      <c r="B12" s="163" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="178" t="s">
+      <c r="C12" s="166" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="179"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="179"/>
-      <c r="G12" s="179"/>
-      <c r="H12" s="179"/>
-      <c r="I12" s="179"/>
-      <c r="J12" s="180"/>
-      <c r="K12" s="178" t="s">
+      <c r="D12" s="167"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="167"/>
+      <c r="J12" s="168"/>
+      <c r="K12" s="166" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="179"/>
-      <c r="M12" s="179"/>
-      <c r="N12" s="179"/>
-      <c r="O12" s="179"/>
-      <c r="P12" s="179"/>
-      <c r="Q12" s="180"/>
-      <c r="R12" s="161" t="s">
+      <c r="L12" s="167"/>
+      <c r="M12" s="167"/>
+      <c r="N12" s="167"/>
+      <c r="O12" s="167"/>
+      <c r="P12" s="167"/>
+      <c r="Q12" s="168"/>
+      <c r="R12" s="169" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="173"/>
-      <c r="B13" s="176"/>
-      <c r="C13" s="164" t="s">
+      <c r="A13" s="161"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="172" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="165"/>
-      <c r="E13" s="165"/>
-      <c r="F13" s="165"/>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="165"/>
-      <c r="J13" s="166"/>
-      <c r="K13" s="164" t="s">
+      <c r="D13" s="173"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="172" t="s">
         <v>134</v>
       </c>
-      <c r="L13" s="165"/>
-      <c r="M13" s="165"/>
-      <c r="N13" s="165"/>
-      <c r="O13" s="165"/>
-      <c r="P13" s="165"/>
-      <c r="Q13" s="166"/>
-      <c r="R13" s="162"/>
+      <c r="L13" s="173"/>
+      <c r="M13" s="173"/>
+      <c r="N13" s="173"/>
+      <c r="O13" s="173"/>
+      <c r="P13" s="173"/>
+      <c r="Q13" s="174"/>
+      <c r="R13" s="170"/>
     </row>
     <row r="14" spans="1:18" ht="25.5">
-      <c r="A14" s="173"/>
-      <c r="B14" s="176"/>
-      <c r="C14" s="167" t="s">
+      <c r="A14" s="161"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="175" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="170" t="s">
+      <c r="D14" s="178" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="170" t="s">
+      <c r="E14" s="178" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="170" t="s">
+      <c r="F14" s="178" t="s">
         <v>138</v>
       </c>
-      <c r="G14" s="167" t="s">
+      <c r="G14" s="175" t="s">
         <v>139</v>
       </c>
-      <c r="H14" s="167" t="s">
+      <c r="H14" s="175" t="s">
         <v>140</v>
       </c>
-      <c r="I14" s="167" t="s">
+      <c r="I14" s="175" t="s">
         <v>141</v>
       </c>
       <c r="J14" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="K14" s="167" t="s">
+      <c r="K14" s="175" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="170" t="s">
+      <c r="L14" s="178" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="170" t="s">
+      <c r="M14" s="178" t="s">
         <v>144</v>
       </c>
-      <c r="N14" s="167" t="s">
+      <c r="N14" s="175" t="s">
         <v>145</v>
       </c>
-      <c r="O14" s="170" t="s">
+      <c r="O14" s="178" t="s">
         <v>146</v>
       </c>
       <c r="P14" s="73" t="s">
@@ -3768,47 +3768,47 @@
       <c r="Q14" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="R14" s="162"/>
+      <c r="R14" s="170"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="173"/>
-      <c r="B15" s="176"/>
-      <c r="C15" s="168"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="171"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="168"/>
-      <c r="H15" s="168"/>
-      <c r="I15" s="168"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="176"/>
+      <c r="D15" s="179"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="179"/>
+      <c r="G15" s="176"/>
+      <c r="H15" s="176"/>
+      <c r="I15" s="176"/>
       <c r="J15" s="72"/>
-      <c r="K15" s="168"/>
-      <c r="L15" s="171"/>
-      <c r="M15" s="171"/>
-      <c r="N15" s="168"/>
-      <c r="O15" s="171"/>
+      <c r="K15" s="176"/>
+      <c r="L15" s="179"/>
+      <c r="M15" s="179"/>
+      <c r="N15" s="176"/>
+      <c r="O15" s="179"/>
       <c r="P15" s="75"/>
       <c r="Q15" s="76"/>
-      <c r="R15" s="162"/>
+      <c r="R15" s="170"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="174"/>
-      <c r="B16" s="177"/>
-      <c r="C16" s="169"/>
-      <c r="D16" s="172"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="172"/>
-      <c r="G16" s="169"/>
-      <c r="H16" s="169"/>
-      <c r="I16" s="169"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="177"/>
       <c r="J16" s="77"/>
-      <c r="K16" s="169"/>
-      <c r="L16" s="172"/>
-      <c r="M16" s="172"/>
-      <c r="N16" s="169"/>
-      <c r="O16" s="172"/>
+      <c r="K16" s="177"/>
+      <c r="L16" s="180"/>
+      <c r="M16" s="180"/>
+      <c r="N16" s="177"/>
+      <c r="O16" s="180"/>
       <c r="P16" s="78"/>
       <c r="Q16" s="79"/>
-      <c r="R16" s="163"/>
+      <c r="R16" s="171"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="80">
@@ -3931,6 +3931,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:J12"/>
@@ -3947,9 +3950,6 @@
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="L14:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3960,8 +3960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6932,10 +6932,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7180,6 +7180,9 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>